<commit_message>
Added skull axis patterns
</commit_message>
<xml_diff>
--- a/terms/skullTerms.xlsx
+++ b/terms/skullTerms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanabalk/GitHub/futres/fovt/terms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\terms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18678180-C91C-914D-A4FC-A8D8A547FD3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B1903A-5958-4763-9C00-EA52AB5C8626}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="14400" windowHeight="16620" xr2:uid="{E38D1147-306F-C442-8001-8D18F9A28679}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{E38D1147-306F-C442-8001-8D18F9A28679}"/>
   </bookViews>
   <sheets>
     <sheet name="trait" sheetId="1" r:id="rId1"/>
@@ -30,173 +30,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={BBF95199-719D-4EFF-9CAC-0AE7D9E53C79}</author>
-    <author>tc={954BEEF1-029F-4B49-9598-7BCB2B8D99C2}</author>
-    <author>tc={E95D16CB-B9FE-4FD3-8E97-8084044FE63A}</author>
-    <author>tc={FFD4E624-BDAA-4E15-BCF5-137D86859ED7}</author>
-    <author>tc={64950143-F985-4890-BE68-D7F105AA86D7}</author>
-    <author>tc={FFADBAE0-0E9E-4C0C-905D-A76BF7A8106A}</author>
-  </authors>
-  <commentList>
-    <comment ref="G86" authorId="0" shapeId="0" xr:uid="{EA8B6FD4-4794-3B40-9C34-F4EFD786758F}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Split into left and right</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G89" authorId="1" shapeId="0" xr:uid="{6E42EA85-FC19-894F-BA8F-880757D1A93D}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Split into left and right</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G93" authorId="2" shapeId="0" xr:uid="{AA6EF430-6B84-A247-AE27-3533812AB0F4}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Split into left and right</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G94" authorId="3" shapeId="0" xr:uid="{B887CCA6-2862-A048-93CD-B270C6E218AD}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Split into left and right</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G104" authorId="4" shapeId="0" xr:uid="{C761E353-4C32-F241-9116-90BAFC57EA14}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Split into left and right</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C128" authorId="5" shapeId="0" xr:uid="{495C85D6-13CD-1E42-B333-5F23E681DB78}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Comment:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">    Should this be internal or external nares?</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
     <author>FuTRES</author>
   </authors>
   <commentList>
-    <comment ref="A63" authorId="0" shapeId="0" xr:uid="{A338449B-C363-824F-8D1C-73EECF37CB5C}">
+    <comment ref="A55" authorId="0" shapeId="0" xr:uid="{A338449B-C363-824F-8D1C-73EECF37CB5C}">
       <text>
         <r>
           <rPr>
@@ -234,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="373">
   <si>
     <t>FOVT STATUS</t>
   </si>
@@ -1326,6 +1163,33 @@
   </si>
   <si>
     <t>line from infraorbital foramen to first molar mesostyle is a proxy for crown height</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'left side' and ('posteriormost part of' some 'occipital condyle')</t>
+  </si>
+  <si>
+    <t>anterior-posterior</t>
+  </si>
+  <si>
+    <t>medial-lateral</t>
+  </si>
+  <si>
+    <t>right side' and (`part of' some 'orbit of skull')</t>
+  </si>
+  <si>
+    <t>left side' and ('part of' some 'orbit of skull')</t>
+  </si>
+  <si>
+    <t>right side' and ('part of' some 'orbit of skull')</t>
+  </si>
+  <si>
+    <t>left side' and ('part of' some 'tetrapod frontal bone')</t>
+  </si>
+  <si>
+    <t>right side' and ('part of' some 'tetrapod frontal bone')</t>
+  </si>
+  <si>
+    <t>upper-lower</t>
   </si>
 </sst>
 </file>
@@ -1462,7 +1326,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1475,13 +1339,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1796,15 +1662,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33FD1B0C-460E-164A-B70B-2EC8726236AE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33FD1B0C-460E-164A-B70B-2EC8726236AE}">
   <dimension ref="A1:Q133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C134" sqref="C134"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
@@ -3989,19 +3855,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DECECE6-49BF-9F4F-B264-E8F452349B07}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="21.375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -4018,6 +3886,94 @@
       </c>
       <c r="E1" t="s">
         <v>270</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="B3" t="s">
+        <v>372</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="B4" t="s">
+        <v>366</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="B5" t="s">
+        <v>366</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="B6" t="s">
+        <v>365</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="B7" t="s">
+        <v>365</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="B8" t="s">
+        <v>366</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="B9" t="s">
+        <v>366</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -4027,13 +3983,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A3F7CC8-7FEA-4649-8303-A7CE04FBC8D5}">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -4053,40 +4009,40 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" customHeight="1">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>207</v>
       </c>
       <c r="B4" t="s">
         <v>277</v>
       </c>
-      <c r="C4" t="s">
-        <v>278</v>
+      <c r="C4" s="11" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>208</v>
       </c>
       <c r="B5" t="s">
@@ -4097,7 +4053,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>209</v>
       </c>
       <c r="B6" t="s">
@@ -4108,7 +4064,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>210</v>
       </c>
       <c r="B7" t="s">
@@ -4119,12 +4075,12 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>212</v>
       </c>
       <c r="B9" t="s">
@@ -4135,12 +4091,12 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>214</v>
       </c>
       <c r="B11" t="s">
@@ -4151,12 +4107,12 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>216</v>
       </c>
       <c r="B13" t="s">
@@ -4167,7 +4123,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="12" t="s">
         <v>217</v>
       </c>
       <c r="B14" t="s">
@@ -4178,7 +4134,7 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="12" t="s">
         <v>218</v>
       </c>
       <c r="B15" t="s">
@@ -4189,7 +4145,7 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>219</v>
       </c>
       <c r="B16" t="s">
@@ -4200,7 +4156,7 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="12" t="s">
         <v>220</v>
       </c>
       <c r="B17" t="s">
@@ -4211,7 +4167,7 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="12" t="s">
         <v>221</v>
       </c>
       <c r="B18" t="s">
@@ -4222,7 +4178,7 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="12" t="s">
         <v>222</v>
       </c>
       <c r="B19" t="s">
@@ -4233,7 +4189,7 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="12" t="s">
         <v>223</v>
       </c>
       <c r="B20" t="s">
@@ -4244,7 +4200,7 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="12" t="s">
         <v>224</v>
       </c>
       <c r="B21" t="s">
@@ -4255,7 +4211,7 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="12" t="s">
         <v>225</v>
       </c>
       <c r="B22" t="s">
@@ -4266,7 +4222,7 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="12" t="s">
         <v>226</v>
       </c>
       <c r="B23" t="s">
@@ -4277,7 +4233,7 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="12" t="s">
         <v>227</v>
       </c>
       <c r="B24" t="s">
@@ -4288,7 +4244,7 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="12" t="s">
         <v>228</v>
       </c>
       <c r="B25" t="s">
@@ -4299,7 +4255,7 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="12" t="s">
         <v>229</v>
       </c>
       <c r="B26" t="s">
@@ -4310,7 +4266,7 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="12" t="s">
         <v>230</v>
       </c>
       <c r="B27" t="s">
@@ -4321,7 +4277,7 @@
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="12" t="s">
         <v>231</v>
       </c>
       <c r="B28" t="s">
@@ -4332,7 +4288,7 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="12" t="s">
         <v>232</v>
       </c>
       <c r="B29" t="s">
@@ -4343,7 +4299,7 @@
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="12" t="s">
         <v>233</v>
       </c>
       <c r="B30" t="s">
@@ -4354,7 +4310,7 @@
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="12" t="s">
         <v>234</v>
       </c>
       <c r="B31" t="s">
@@ -4365,7 +4321,7 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="12" t="s">
         <v>235</v>
       </c>
       <c r="B32" t="s">
@@ -4376,7 +4332,7 @@
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="12" t="s">
         <v>236</v>
       </c>
       <c r="B33" t="s">
@@ -4387,7 +4343,7 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="12" t="s">
         <v>237</v>
       </c>
       <c r="B34" t="s">
@@ -4398,7 +4354,7 @@
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="13" t="s">
         <v>207</v>
       </c>
       <c r="B35" t="s">
@@ -4409,18 +4365,18 @@
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="13" t="s">
         <v>238</v>
       </c>
       <c r="B36" t="s">
         <v>326</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C36" s="14" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="13" t="s">
         <v>239</v>
       </c>
       <c r="B37" t="s">
@@ -4431,7 +4387,7 @@
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="13" t="s">
         <v>240</v>
       </c>
       <c r="B38" t="s">
@@ -4442,7 +4398,7 @@
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="13" t="s">
         <v>241</v>
       </c>
       <c r="B39" t="s">
@@ -4453,34 +4409,34 @@
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="14" t="s">
         <v>334</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="14" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="13" t="s">
         <v>243</v>
       </c>
       <c r="B41" t="s">
         <v>336</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="14" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="14" t="s">
+      <c r="A42" s="13" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="13" t="s">
         <v>245</v>
       </c>
       <c r="B43" t="s">
@@ -4491,7 +4447,7 @@
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="13" t="s">
         <v>246</v>
       </c>
       <c r="B44" t="s">
@@ -4502,7 +4458,7 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="13" t="s">
         <v>247</v>
       </c>
       <c r="B45" t="s">
@@ -4513,7 +4469,7 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="14" t="s">
+      <c r="A46" s="13" t="s">
         <v>248</v>
       </c>
       <c r="B46" t="s">
@@ -4524,7 +4480,7 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="13" t="s">
         <v>249</v>
       </c>
       <c r="B47" t="s">
@@ -4535,10 +4491,10 @@
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="14" t="s">
+      <c r="A48" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="14" t="s">
         <v>347</v>
       </c>
       <c r="C48" t="s">
@@ -4546,10 +4502,10 @@
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="B49" s="14" t="s">
         <v>347</v>
       </c>
       <c r="C49" t="s">
@@ -4557,7 +4513,7 @@
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="14" t="s">
+      <c r="A50" s="13" t="s">
         <v>252</v>
       </c>
       <c r="B50" t="s">
@@ -4568,18 +4524,18 @@
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="14" t="s">
+      <c r="A51" s="13" t="s">
         <v>253</v>
       </c>
       <c r="B51" t="s">
         <v>352</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="C51" s="14" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="14" t="s">
+      <c r="A52" s="13" t="s">
         <v>254</v>
       </c>
       <c r="B52" t="s">
@@ -4590,69 +4546,29 @@
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="14" t="s">
-        <v>255</v>
+      <c r="A53" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="B53" t="s">
+        <v>356</v>
+      </c>
+      <c r="C53" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="14" t="s">
-        <v>256</v>
+      <c r="A54" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="14" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="14" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="14" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="14" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B59" t="s">
-        <v>356</v>
-      </c>
-      <c r="C59" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="16" t="s">
-        <v>262</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="14" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="14" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="14" t="s">
+      <c r="A55" s="13" t="s">
         <v>265</v>
       </c>
     </row>
@@ -4670,7 +4586,7 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Added skull AB patterns
</commit_message>
<xml_diff>
--- a/terms/skullTerms.xlsx
+++ b/terms/skullTerms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\terms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B1903A-5958-4763-9C00-EA52AB5C8626}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E9C037-2897-4AA7-9FB8-A79B895318B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{E38D1147-306F-C442-8001-8D18F9A28679}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="372">
   <si>
     <t>FOVT STATUS</t>
   </si>
@@ -1123,36 +1123,12 @@
     <t>Anterior-most border of internal nares</t>
   </si>
   <si>
-    <t>Posterior-most border of left internal nares</t>
-  </si>
-  <si>
-    <t>Posterior-most extent of left occipital condyle</t>
-  </si>
-  <si>
     <t>Right lateral midpoint of orbital length</t>
   </si>
   <si>
     <t>Left lateral midpoint of orbital length</t>
   </si>
   <si>
-    <t>Right postorbital process</t>
-  </si>
-  <si>
-    <t>Left postorbital process</t>
-  </si>
-  <si>
-    <t>Anterior-most extent of palatine at midline</t>
-  </si>
-  <si>
-    <t>Posterior-most extent of palatine at midline</t>
-  </si>
-  <si>
-    <t>Right lateral-most extent of nares</t>
-  </si>
-  <si>
-    <t>Left lateral-most extent of nares</t>
-  </si>
-  <si>
     <t>axis</t>
   </si>
   <si>
@@ -1190,6 +1166,27 @@
   </si>
   <si>
     <t>upper-lower</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'left side' and ('lateralmost part of' some 'postorbital process')</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'right side' and ('lateralmost part of' some 'postorbital process')</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'medial side' and ('anteriormost part of' some 'palatine bone')</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'medial side' and ('posteriormost part of' some 'palatine bone')</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'left side' and ('lateralmost part of' some 'external naris')</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'right side' and ('lateralmost part of' some 'external naris')</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'left side' and ('posteriormost part of' some 'internal naris')</t>
   </si>
 </sst>
 </file>
@@ -1269,7 +1266,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1306,12 +1303,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1326,7 +1317,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1344,7 +1335,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1666,8 +1656,8 @@
   <dimension ref="A1:Q133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K40" sqref="K40"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3847,10 +3837,10 @@
     </row>
     <row r="133" spans="3:9">
       <c r="C133" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="I133" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -3863,7 +3853,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3876,10 +3866,10 @@
         <v>267</v>
       </c>
       <c r="B1" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C1" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D1" t="s">
         <v>101</v>
@@ -3889,91 +3879,91 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>255</v>
       </c>
       <c r="B2" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>256</v>
       </c>
       <c r="B3" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>257</v>
       </c>
       <c r="B4" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>258</v>
       </c>
       <c r="B5" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>259</v>
       </c>
       <c r="B6" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>260</v>
       </c>
       <c r="B7" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>263</v>
       </c>
       <c r="B8" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>264</v>
       </c>
       <c r="B9" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -3983,10 +3973,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A3F7CC8-7FEA-4649-8303-A7CE04FBC8D5}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4009,7 +3999,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" customHeight="1">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>271</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -4020,7 +4010,7 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>274</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -4038,7 +4028,7 @@
         <v>277</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4513,14 +4503,14 @@
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="B50" t="s">
-        <v>350</v>
-      </c>
-      <c r="C50" t="s">
-        <v>351</v>
+      <c r="B50" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -4528,49 +4518,57 @@
         <v>253</v>
       </c>
       <c r="B51" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="13" t="s">
+      <c r="A52" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="B52" t="s">
-        <v>354</v>
-      </c>
-      <c r="C52" t="s">
-        <v>355</v>
+      <c r="B52" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="13" t="s">
+      <c r="A53" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="B53" t="s">
-        <v>356</v>
-      </c>
-      <c r="C53" t="s">
-        <v>357</v>
+      <c r="B53" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="15" t="s">
+      <c r="A54" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="B54" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>359</v>
+      <c r="B54" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="13" t="s">
         <v>265</v>
       </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added AB patterns and small edits
</commit_message>
<xml_diff>
--- a/terms/skullTerms.xlsx
+++ b/terms/skullTerms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\terms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84915BB0-B610-4E60-9CE3-EEEE8BD63D78}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10D8645-05AD-42D8-B3C1-2F9971D9BF21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{E38D1147-306F-C442-8001-8D18F9A28679}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="2" xr2:uid="{E38D1147-306F-C442-8001-8D18F9A28679}"/>
   </bookViews>
   <sheets>
     <sheet name="trait" sheetId="1" r:id="rId1"/>
@@ -30,21 +30,32 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={1E6A4276-088D-4855-B32A-DC10C0B66366}</author>
+    <author>tc={C6D674AA-10AC-4CF3-8DEC-641DB61E7179}</author>
+    <author>tc={F1BD5B78-17AC-4443-B2FA-D08EDB39FDF9}</author>
     <author>tc={347C81A4-21AC-4EEA-B6E2-B4A8455C8C45}</author>
     <author>tc={A8EE68F2-714F-4653-9C5C-C7347112CF21}</author>
     <author>FuTRES</author>
   </authors>
   <commentList>
-    <comment ref="C18" authorId="0" shapeId="0" xr:uid="{1E6A4276-088D-4855-B32A-DC10C0B66366}">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{C6D674AA-10AC-4CF3-8DEC-641DB61E7179}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    'anatomical point' and 'left side' and ('posteriormost part of' some 'alveolar ridge')</t>
+    'anatomical point' and ('anteriormost part of' some 'premaxilla')
+Reply:
+    use rostrum</t>
       </text>
     </comment>
-    <comment ref="B43" authorId="1" shapeId="0" xr:uid="{347C81A4-21AC-4EEA-B6E2-B4A8455C8C45}">
+    <comment ref="B22" authorId="1" shapeId="0" xr:uid="{F1BD5B78-17AC-4443-B2FA-D08EDB39FDF9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    'anatomical point' and 'left side' and ('antero-ventral margin' some 'infra-orbital foramen of maxilla')</t>
+      </text>
+    </comment>
+    <comment ref="B43" authorId="2" shapeId="0" xr:uid="{347C81A4-21AC-4EEA-B6E2-B4A8455C8C45}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -52,7 +63,7 @@
     'anatomical point' and 'left side' and ('posteriormost part of' and 'lateralmost part of' some 'nasal bone')</t>
       </text>
     </comment>
-    <comment ref="C43" authorId="2" shapeId="0" xr:uid="{A8EE68F2-714F-4653-9C5C-C7347112CF21}">
+    <comment ref="C43" authorId="3" shapeId="0" xr:uid="{A8EE68F2-714F-4653-9C5C-C7347112CF21}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -60,7 +71,7 @@
     'anatomical point' and 'left side' and ('anteriormost part of' and 'lateralmost part of' some 'nasal bone')</t>
       </text>
     </comment>
-    <comment ref="A55" authorId="3" shapeId="0" xr:uid="{A338449B-C363-824F-8D1C-73EECF37CB5C}">
+    <comment ref="A55" authorId="4" shapeId="0" xr:uid="{A338449B-C363-824F-8D1C-73EECF37CB5C}">
       <text>
         <r>
           <rPr>
@@ -98,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="380">
   <si>
     <t>FOVT STATUS</t>
   </si>
@@ -961,15 +972,6 @@
     <t>Palatal notch</t>
   </si>
   <si>
-    <t>Posterior-most extent of left posterior-most alveolus</t>
-  </si>
-  <si>
-    <t>Posteriormost extent of right canine alveolus</t>
-  </si>
-  <si>
-    <t>Posterior-most extent of right posterior-most alveolus</t>
-  </si>
-  <si>
     <t>Left lateral-most extent of rostrum at level of posteriormost extent of left canine alveolus</t>
   </si>
   <si>
@@ -991,12 +993,6 @@
     <t>Anteroventral extent of right orbit</t>
   </si>
   <si>
-    <t>Medial wall of left posterior lacerate foramen</t>
-  </si>
-  <si>
-    <t>Medial wall of right posterior lacerate foramen</t>
-  </si>
-  <si>
     <t>Midpoint of the width of the alveoli for left P2 and P3</t>
   </si>
   <si>
@@ -1195,9 +1191,6 @@
     <t>anatomical point' and 'right side' and 'dorsal side' and ('lateralmost part of' some 'premaxilla')</t>
   </si>
   <si>
-    <t>anatomical point' and 'left side' and ('posteriormost part of' some 'tooth socket' and 'upper canine 1')</t>
-  </si>
-  <si>
     <t>anatomical point' and 'left side' and ('lateralmost part of' some 'anterior naris')</t>
   </si>
   <si>
@@ -1220,13 +1213,49 @@
   </si>
   <si>
     <t>anatomical point' and 'right side' and ('lateralmost part of' some 'nasal bone')</t>
+  </si>
+  <si>
+    <t>Upper left canine to posterior-most alveolus</t>
+  </si>
+  <si>
+    <t>Upper right canine to posterior-most alveolus</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'left side' and ('medialmost part of' some 'jugular foramen')</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'right side' and ('medialmost part of' some 'jugular foramen')</t>
+  </si>
+  <si>
+    <t>preorbital process</t>
+  </si>
+  <si>
+    <t>Can this be defined using logic?</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'left side' and ('posteriormost part of' some 'tooth socket' ('part of' some 'upper canine 1')</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'left side' and ('posteriormost part of' some 'tooth socket' ('part of' some 'upper tooth row')</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'right side' and ('posteriormost part of' some 'tooth socket' ('part of' some 'upper canine 1')</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'right side' and ('posteriormost part of' some 'tooth socket' ('part of' some 'upper tooth row')</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'left side' and ('anteriormost part of' some 'tooth socket' ('part of' some 'upper tooth row')</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'right side' and ('anteriormost part of' some 'tooth socket' ('part of' some 'upper tooth row')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1303,6 +1332,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1698,8 +1733,14 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C18" dT="2021-05-21T20:06:58.81" personId="{51C475B7-EA5B-45B0-A5F6-77D42C7C2A1F}" id="{1E6A4276-088D-4855-B32A-DC10C0B66366}">
-    <text>'anatomical point' and 'left side' and ('posteriormost part of' some 'alveolar ridge')</text>
+  <threadedComment ref="B4" dT="2021-05-24T16:49:34.22" personId="{51C475B7-EA5B-45B0-A5F6-77D42C7C2A1F}" id="{C6D674AA-10AC-4CF3-8DEC-641DB61E7179}">
+    <text>'anatomical point' and ('anteriormost part of' some 'premaxilla')</text>
+  </threadedComment>
+  <threadedComment ref="B4" dT="2021-05-24T18:12:27.60" personId="{51C475B7-EA5B-45B0-A5F6-77D42C7C2A1F}" id="{9F3B3E3D-13B8-4379-8281-5AF4D863E9E6}" parentId="{C6D674AA-10AC-4CF3-8DEC-641DB61E7179}">
+    <text>use rostrum</text>
+  </threadedComment>
+  <threadedComment ref="B22" dT="2021-05-24T17:18:28.37" personId="{51C475B7-EA5B-45B0-A5F6-77D42C7C2A1F}" id="{F1BD5B78-17AC-4443-B2FA-D08EDB39FDF9}">
+    <text>'anatomical point' and 'left side' and ('antero-ventral margin' some 'infra-orbital foramen of maxilla')</text>
   </threadedComment>
   <threadedComment ref="B43" dT="2021-05-21T20:53:29.44" personId="{51C475B7-EA5B-45B0-A5F6-77D42C7C2A1F}" id="{347C81A4-21AC-4EEA-B6E2-B4A8455C8C45}">
     <text>'anatomical point' and 'left side' and ('posteriormost part of' and 'lateralmost part of' some 'nasal bone')</text>
@@ -1715,7 +1756,7 @@
   <dimension ref="A1:Q133"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
@@ -3896,10 +3937,10 @@
     </row>
     <row r="133" spans="3:9">
       <c r="C133" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I133" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -3909,10 +3950,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DECECE6-49BF-9F4F-B264-E8F452349B07}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C11" sqref="C10:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3920,15 +3961,15 @@
     <col min="1" max="1" width="21.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>267</v>
       </c>
       <c r="B1" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="C1" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D1" t="s">
         <v>101</v>
@@ -3937,93 +3978,100 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" s="16" t="s">
         <v>255</v>
       </c>
       <c r="B2" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="16" t="s">
         <v>256</v>
       </c>
       <c r="B3" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="16" t="s">
         <v>257</v>
       </c>
       <c r="B4" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="16" t="s">
         <v>258</v>
       </c>
       <c r="B5" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="16" t="s">
         <v>259</v>
       </c>
       <c r="B6" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="16" t="s">
         <v>260</v>
       </c>
       <c r="B7" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="16" t="s">
         <v>263</v>
       </c>
       <c r="B8" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="16" t="s">
         <v>264</v>
       </c>
       <c r="B9" t="s">
+        <v>340</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>350</v>
-      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="C10" s="10"/>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="C11" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4034,8 +4082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A3F7CC8-7FEA-4649-8303-A7CE04FBC8D5}">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4080,14 +4128,14 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="17" t="s">
         <v>207</v>
       </c>
       <c r="B4" t="s">
         <v>277</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4128,10 +4176,10 @@
         <v>211</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4155,10 +4203,10 @@
         <v>214</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="G11" s="10"/>
     </row>
@@ -4172,10 +4220,10 @@
         <v>216</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -4183,10 +4231,10 @@
         <v>217</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -4197,7 +4245,7 @@
         <v>284</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -4208,7 +4256,7 @@
         <v>284</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -4223,37 +4271,36 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="17" t="s">
-        <v>221</v>
+      <c r="A18" s="15" t="s">
+        <v>368</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>365</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>287</v>
-      </c>
-      <c r="G18" s="10"/>
+        <v>374</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="B19" t="s">
-        <v>288</v>
-      </c>
-      <c r="C19" t="s">
-        <v>289</v>
+      <c r="A19" s="15" t="s">
+        <v>369</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="B20" t="s">
-        <v>290</v>
-      </c>
-      <c r="C20" t="s">
-        <v>291</v>
+      <c r="B20" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -4264,40 +4311,41 @@
         <v>277</v>
       </c>
       <c r="C21" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="B22" t="s">
-        <v>293</v>
+      <c r="B22" s="17" t="s">
+        <v>290</v>
       </c>
       <c r="C22" t="s">
-        <v>294</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F22" s="10"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="11" t="s">
         <v>226</v>
       </c>
       <c r="B23" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C23" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="B24" t="s">
-        <v>297</v>
-      </c>
-      <c r="C24" t="s">
-        <v>298</v>
+      <c r="B24" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -4305,10 +4353,10 @@
         <v>228</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
@@ -4318,10 +4366,10 @@
         <v>229</v>
       </c>
       <c r="B26" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C26" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -4329,10 +4377,10 @@
         <v>230</v>
       </c>
       <c r="B27" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="C27" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -4340,10 +4388,10 @@
         <v>231</v>
       </c>
       <c r="B28" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="C28" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -4351,10 +4399,10 @@
         <v>232</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -4362,10 +4410,10 @@
         <v>233</v>
       </c>
       <c r="B30" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C30" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -4373,10 +4421,10 @@
         <v>234</v>
       </c>
       <c r="B31" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C31" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -4384,10 +4432,10 @@
         <v>235</v>
       </c>
       <c r="B32" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="C32" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -4395,10 +4443,10 @@
         <v>236</v>
       </c>
       <c r="B33" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C33" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -4406,10 +4454,10 @@
         <v>237</v>
       </c>
       <c r="B34" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C34" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -4417,7 +4465,7 @@
         <v>207</v>
       </c>
       <c r="B35" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="C35" t="s">
         <v>278</v>
@@ -4428,10 +4476,10 @@
         <v>238</v>
       </c>
       <c r="B36" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -4439,10 +4487,10 @@
         <v>239</v>
       </c>
       <c r="B37" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="C37" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -4450,10 +4498,10 @@
         <v>240</v>
       </c>
       <c r="B38" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C38" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -4461,10 +4509,10 @@
         <v>241</v>
       </c>
       <c r="B39" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C39" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -4472,10 +4520,10 @@
         <v>242</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -4483,10 +4531,10 @@
         <v>243</v>
       </c>
       <c r="B41" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -4494,10 +4542,10 @@
         <v>244</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="F42" s="10"/>
     </row>
@@ -4506,10 +4554,10 @@
         <v>245</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
@@ -4519,10 +4567,10 @@
         <v>246</v>
       </c>
       <c r="B44" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C44" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -4530,10 +4578,10 @@
         <v>247</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -4541,10 +4589,10 @@
         <v>248</v>
       </c>
       <c r="B46" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="C46" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -4552,10 +4600,10 @@
         <v>249</v>
       </c>
       <c r="B47" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="C47" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -4563,10 +4611,10 @@
         <v>250</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C48" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -4574,10 +4622,10 @@
         <v>251</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C49" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -4585,10 +4633,10 @@
         <v>252</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -4596,10 +4644,10 @@
         <v>253</v>
       </c>
       <c r="B51" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -4607,10 +4655,10 @@
         <v>254</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -4618,10 +4666,10 @@
         <v>261</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -4629,10 +4677,10 @@
         <v>262</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -4640,9 +4688,27 @@
         <v>265</v>
       </c>
     </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>378</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>375</v>
+      </c>
+    </row>
     <row r="57" spans="1:3">
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
+      <c r="A57" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="58" spans="1:3">
       <c r="B58" s="10"/>
@@ -4650,16 +4716,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA6A50E-5517-0B4F-B6AB-1E94580FA579}">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4824,24 +4891,32 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="3:3">
+    <row r="17" spans="3:12">
       <c r="C17" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="3:3">
+    <row r="18" spans="3:12">
       <c r="C18" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="3:3">
+    <row r="19" spans="3:12">
       <c r="C19" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="3:3">
+    <row r="20" spans="3:12">
       <c r="C20" s="3" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12">
+      <c r="C21" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="L21" t="s">
+        <v>373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added rostrum AB patterns
</commit_message>
<xml_diff>
--- a/terms/skullTerms.xlsx
+++ b/terms/skullTerms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\terms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10D8645-05AD-42D8-B3C1-2F9971D9BF21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97440D1E-5107-48D8-BCB6-A7A836887D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="2" xr2:uid="{E38D1147-306F-C442-8001-8D18F9A28679}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{E38D1147-306F-C442-8001-8D18F9A28679}"/>
   </bookViews>
   <sheets>
     <sheet name="trait" sheetId="1" r:id="rId1"/>
@@ -30,32 +30,12 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={C6D674AA-10AC-4CF3-8DEC-641DB61E7179}</author>
-    <author>tc={F1BD5B78-17AC-4443-B2FA-D08EDB39FDF9}</author>
     <author>tc={347C81A4-21AC-4EEA-B6E2-B4A8455C8C45}</author>
     <author>tc={A8EE68F2-714F-4653-9C5C-C7347112CF21}</author>
     <author>FuTRES</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{C6D674AA-10AC-4CF3-8DEC-641DB61E7179}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    'anatomical point' and ('anteriormost part of' some 'premaxilla')
-Reply:
-    use rostrum</t>
-      </text>
-    </comment>
-    <comment ref="B22" authorId="1" shapeId="0" xr:uid="{F1BD5B78-17AC-4443-B2FA-D08EDB39FDF9}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    'anatomical point' and 'left side' and ('antero-ventral margin' some 'infra-orbital foramen of maxilla')</t>
-      </text>
-    </comment>
-    <comment ref="B43" authorId="2" shapeId="0" xr:uid="{347C81A4-21AC-4EEA-B6E2-B4A8455C8C45}">
+    <comment ref="B43" authorId="0" shapeId="0" xr:uid="{347C81A4-21AC-4EEA-B6E2-B4A8455C8C45}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -63,7 +43,7 @@
     'anatomical point' and 'left side' and ('posteriormost part of' and 'lateralmost part of' some 'nasal bone')</t>
       </text>
     </comment>
-    <comment ref="C43" authorId="3" shapeId="0" xr:uid="{A8EE68F2-714F-4653-9C5C-C7347112CF21}">
+    <comment ref="C43" authorId="1" shapeId="0" xr:uid="{A8EE68F2-714F-4653-9C5C-C7347112CF21}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -71,7 +51,7 @@
     'anatomical point' and 'left side' and ('anteriormost part of' and 'lateralmost part of' some 'nasal bone')</t>
       </text>
     </comment>
-    <comment ref="A55" authorId="4" shapeId="0" xr:uid="{A338449B-C363-824F-8D1C-73EECF37CB5C}">
+    <comment ref="A55" authorId="2" shapeId="0" xr:uid="{A338449B-C363-824F-8D1C-73EECF37CB5C}">
       <text>
         <r>
           <rPr>
@@ -109,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="379">
   <si>
     <t>FOVT STATUS</t>
   </si>
@@ -942,9 +922,6 @@
     <t>anatomical point' and ('anteriormost part of' some 'foramen magnum')</t>
   </si>
   <si>
-    <t>Anteriormost extent of rostrum</t>
-  </si>
-  <si>
     <t>Posterior margin of left occipital condyle</t>
   </si>
   <si>
@@ -981,18 +958,6 @@
     <t>Midline of level of posterior extent of maxillae</t>
   </si>
   <si>
-    <t>Anteroventral extent of left infraorbital foramen</t>
-  </si>
-  <si>
-    <t>Anteroventral extent of left orbit</t>
-  </si>
-  <si>
-    <t>Anteroventral extent of right infraorbital foramen</t>
-  </si>
-  <si>
-    <t>Anteroventral extent of right orbit</t>
-  </si>
-  <si>
     <t>Midpoint of the width of the alveoli for left P2 and P3</t>
   </si>
   <si>
@@ -1017,12 +982,6 @@
     <t>Midpoint of the width of the palate directly dorsal to midpoint of imaginary line</t>
   </si>
   <si>
-    <t>Left eustachian/auditory tube</t>
-  </si>
-  <si>
-    <t>Right eustachian/auditory tube</t>
-  </si>
-  <si>
     <t>Dorsal intercondylar notch</t>
   </si>
   <si>
@@ -1041,9 +1000,6 @@
     <t>Posterior surface of the right paraoccipital</t>
   </si>
   <si>
-    <t>Anterior-most extent of rostrum</t>
-  </si>
-  <si>
     <t>antorbital notches</t>
   </si>
   <si>
@@ -1249,13 +1205,34 @@
   </si>
   <si>
     <t>anatomical point' and 'right side' and ('anteriormost part of' some 'tooth socket' ('part of' some 'upper tooth row')</t>
+  </si>
+  <si>
+    <t>anatomical point' and ('anteriormost part of' some 'rostrum')</t>
+  </si>
+  <si>
+    <t>'anatomical point' and 'left side' and ('antero-ventral margin' some 'infra-orbital foramen of maxilla')</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'left side' and ('antero-ventral margin' some 'orbit of skull')</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'right side' and ('antero-ventral margin' some 'infra-orbital foramen of maxilla')</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'right side' and ('antero-ventral margin' some 'orbit of skull')</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'left side' and ('lateralmost part of' some 'bony part of pharyngotympanic tube')</t>
+  </si>
+  <si>
+    <t>anatomical point' and 'right side' and ('lateralmost part of' some 'bony part of pharyngotympanic tube')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1327,18 +1304,6 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1391,7 +1356,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1412,6 +1377,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1733,15 +1705,6 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B4" dT="2021-05-24T16:49:34.22" personId="{51C475B7-EA5B-45B0-A5F6-77D42C7C2A1F}" id="{C6D674AA-10AC-4CF3-8DEC-641DB61E7179}">
-    <text>'anatomical point' and ('anteriormost part of' some 'premaxilla')</text>
-  </threadedComment>
-  <threadedComment ref="B4" dT="2021-05-24T18:12:27.60" personId="{51C475B7-EA5B-45B0-A5F6-77D42C7C2A1F}" id="{9F3B3E3D-13B8-4379-8281-5AF4D863E9E6}" parentId="{C6D674AA-10AC-4CF3-8DEC-641DB61E7179}">
-    <text>use rostrum</text>
-  </threadedComment>
-  <threadedComment ref="B22" dT="2021-05-24T17:18:28.37" personId="{51C475B7-EA5B-45B0-A5F6-77D42C7C2A1F}" id="{F1BD5B78-17AC-4443-B2FA-D08EDB39FDF9}">
-    <text>'anatomical point' and 'left side' and ('antero-ventral margin' some 'infra-orbital foramen of maxilla')</text>
-  </threadedComment>
   <threadedComment ref="B43" dT="2021-05-21T20:53:29.44" personId="{51C475B7-EA5B-45B0-A5F6-77D42C7C2A1F}" id="{347C81A4-21AC-4EEA-B6E2-B4A8455C8C45}">
     <text>'anatomical point' and 'left side' and ('posteriormost part of' and 'lateralmost part of' some 'nasal bone')</text>
   </threadedComment>
@@ -3937,10 +3900,10 @@
     </row>
     <row r="133" spans="3:9">
       <c r="C133" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="I133" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -3966,10 +3929,10 @@
         <v>267</v>
       </c>
       <c r="B1" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="C1" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="D1" t="s">
         <v>101</v>
@@ -3983,10 +3946,10 @@
         <v>255</v>
       </c>
       <c r="B2" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -3994,10 +3957,10 @@
         <v>256</v>
       </c>
       <c r="B3" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -4005,10 +3968,10 @@
         <v>257</v>
       </c>
       <c r="B4" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4016,10 +3979,10 @@
         <v>258</v>
       </c>
       <c r="B5" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4027,10 +3990,10 @@
         <v>259</v>
       </c>
       <c r="B6" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4038,10 +4001,10 @@
         <v>260</v>
       </c>
       <c r="B7" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4049,10 +4012,10 @@
         <v>263</v>
       </c>
       <c r="B8" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4060,10 +4023,10 @@
         <v>264</v>
       </c>
       <c r="B9" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -4082,8 +4045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A3F7CC8-7FEA-4649-8303-A7CE04FBC8D5}">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4128,36 +4091,36 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="B4" t="s">
-        <v>277</v>
+      <c r="B4" s="19" t="s">
+        <v>372</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B5" t="s">
-        <v>277</v>
+      <c r="B5" s="19" t="s">
+        <v>372</v>
       </c>
       <c r="C5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="B6" t="s">
-        <v>277</v>
+      <c r="B6" s="19" t="s">
+        <v>372</v>
       </c>
       <c r="C6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4165,10 +4128,10 @@
         <v>210</v>
       </c>
       <c r="B7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4176,10 +4139,10 @@
         <v>211</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4187,10 +4150,10 @@
         <v>212</v>
       </c>
       <c r="B9" t="s">
+        <v>281</v>
+      </c>
+      <c r="C9" t="s">
         <v>282</v>
-      </c>
-      <c r="C9" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -4203,10 +4166,10 @@
         <v>214</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="G11" s="10"/>
     </row>
@@ -4220,10 +4183,10 @@
         <v>216</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -4231,10 +4194,10 @@
         <v>217</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -4242,10 +4205,10 @@
         <v>218</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -4253,10 +4216,10 @@
         <v>219</v>
       </c>
       <c r="B16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -4264,32 +4227,32 @@
         <v>220</v>
       </c>
       <c r="B17" t="s">
+        <v>284</v>
+      </c>
+      <c r="C17" t="s">
         <v>285</v>
-      </c>
-      <c r="C17" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="15" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="15" t="s">
+        <v>361</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>369</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -4297,44 +4260,44 @@
         <v>223</v>
       </c>
       <c r="B20" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>287</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="B21" t="s">
-        <v>277</v>
+      <c r="B21" s="19" t="s">
+        <v>372</v>
       </c>
       <c r="C21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="B22" s="17" t="s">
-        <v>290</v>
-      </c>
-      <c r="C22" t="s">
-        <v>291</v>
+      <c r="B22" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>374</v>
       </c>
       <c r="F22" s="10"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="B23" t="s">
-        <v>292</v>
-      </c>
-      <c r="C23" t="s">
-        <v>293</v>
+      <c r="B23" s="19" t="s">
+        <v>375</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -4342,10 +4305,10 @@
         <v>227</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -4353,10 +4316,10 @@
         <v>228</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
@@ -4366,10 +4329,10 @@
         <v>229</v>
       </c>
       <c r="B26" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C26" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -4377,10 +4340,10 @@
         <v>230</v>
       </c>
       <c r="B27" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C27" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -4388,10 +4351,10 @@
         <v>231</v>
       </c>
       <c r="B28" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="C28" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -4399,10 +4362,10 @@
         <v>232</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -4410,21 +4373,21 @@
         <v>233</v>
       </c>
       <c r="B30" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C30" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="15" t="s">
         <v>234</v>
       </c>
-      <c r="B31" t="s">
-        <v>302</v>
-      </c>
-      <c r="C31" t="s">
-        <v>303</v>
+      <c r="B31" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -4432,10 +4395,10 @@
         <v>235</v>
       </c>
       <c r="B32" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="C32" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -4443,10 +4406,10 @@
         <v>236</v>
       </c>
       <c r="B33" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="C33" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -4454,32 +4417,32 @@
         <v>237</v>
       </c>
       <c r="B34" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="C34" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="B35" t="s">
-        <v>310</v>
+      <c r="B35" s="19" t="s">
+        <v>372</v>
       </c>
       <c r="C35" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="B36" t="s">
-        <v>310</v>
+      <c r="B36" s="19" t="s">
+        <v>372</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -4487,10 +4450,10 @@
         <v>239</v>
       </c>
       <c r="B37" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="C37" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -4498,10 +4461,10 @@
         <v>240</v>
       </c>
       <c r="B38" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="C38" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -4509,10 +4472,10 @@
         <v>241</v>
       </c>
       <c r="B39" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="C39" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -4520,10 +4483,10 @@
         <v>242</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -4531,10 +4494,10 @@
         <v>243</v>
       </c>
       <c r="B41" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -4542,10 +4505,10 @@
         <v>244</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="F42" s="10"/>
     </row>
@@ -4554,10 +4517,10 @@
         <v>245</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
@@ -4567,10 +4530,10 @@
         <v>246</v>
       </c>
       <c r="B44" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="C44" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -4578,10 +4541,10 @@
         <v>247</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -4589,10 +4552,10 @@
         <v>248</v>
       </c>
       <c r="B46" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="C46" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -4600,10 +4563,10 @@
         <v>249</v>
       </c>
       <c r="B47" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="C47" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -4611,10 +4574,10 @@
         <v>250</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="C48" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -4622,10 +4585,10 @@
         <v>251</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="C49" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -4633,10 +4596,10 @@
         <v>252</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -4644,10 +4607,10 @@
         <v>253</v>
       </c>
       <c r="B51" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -4655,10 +4618,10 @@
         <v>254</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -4666,10 +4629,10 @@
         <v>261</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -4677,10 +4640,10 @@
         <v>262</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -4693,10 +4656,10 @@
         <v>221</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -4704,10 +4667,10 @@
         <v>222</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -4913,10 +4876,10 @@
     </row>
     <row r="21" spans="3:12">
       <c r="C21" s="3" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="L21" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Highlighted term and small edits
</commit_message>
<xml_diff>
--- a/terms/skullTerms.xlsx
+++ b/terms/skullTerms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanabalk/GitHub/futres/fovt/terms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\terms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5096ABF5-A606-3A49-B815-44BEC6D6A084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB3815B-AC2F-45C0-9419-72EBB9962D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="580" windowWidth="14400" windowHeight="16620" activeTab="2" xr2:uid="{E38D1147-306F-C442-8001-8D18F9A28679}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="2" xr2:uid="{E38D1147-306F-C442-8001-8D18F9A28679}"/>
   </bookViews>
   <sheets>
     <sheet name="trait" sheetId="1" r:id="rId1"/>
@@ -63,33 +63,6 @@
             <family val="2"/>
           </rPr>
           <t>Check and compare these</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={9CD61875-0363-454F-A529-76F93DDD93EB}</author>
-  </authors>
-  <commentList>
-    <comment ref="A36" authorId="0" shapeId="0" xr:uid="{C8116C2F-8323-0E48-B331-27048A5F3DB4}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Not sure if this could just be reformatted as an axis patter (anterior-posterior axis, 'part of' some 'rostrum'). "antorbital notch' needs to be added to uberon.</t>
         </r>
       </text>
     </comment>
@@ -1339,7 +1312,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1364,6 +1337,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1378,7 +1357,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1403,6 +1382,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1422,9 +1402,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Amanda Peng" id="{51C475B7-EA5B-45B0-A5F6-77D42C7C2A1F}" userId="Amanda Peng" providerId="None"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1722,17 +1700,6 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B43" dT="2021-05-21T20:53:29.44" personId="{51C475B7-EA5B-45B0-A5F6-77D42C7C2A1F}" id="{347C81A4-21AC-4EEA-B6E2-B4A8455C8C45}">
-    <text>'anatomical point' and 'left side' and ('posteriormost part of' and 'lateralmost part of' some 'nasal bone')</text>
-  </threadedComment>
-  <threadedComment ref="C43" dT="2021-05-21T20:53:41.61" personId="{51C475B7-EA5B-45B0-A5F6-77D42C7C2A1F}" id="{A8EE68F2-714F-4653-9C5C-C7347112CF21}">
-    <text>'anatomical point' and 'left side' and ('anteriormost part of' and 'lateralmost part of' some 'nasal bone')</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33FD1B0C-460E-164A-B70B-2EC8726236AE}">
   <dimension ref="A1:Q133"/>
@@ -1742,7 +1709,7 @@
       <selection pane="bottomLeft" activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
@@ -3935,12 +3902,12 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.3125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -4070,14 +4037,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A3F7CC8-7FEA-4649-8303-A7CE04FBC8D5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A3F7CC8-7FEA-4649-8303-A7CE04FBC8D5}">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -4284,7 +4251,7 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="18" t="s">
         <v>204</v>
       </c>
       <c r="B20" t="s">
@@ -4688,7 +4655,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4697,10 +4663,10 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">

</xml_diff>